<commit_message>
Add test, new pet, and new logic for titles
In ApiDataRequest when I am searching for which title is equipped I
added a check to make title = to a empty string so that the character
name is just shown.
</commit_message>
<xml_diff>
--- a/src/main/resources/battlepets.xlsx
+++ b/src/main/resources/battlepets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\eclipse-workspace\BingeWolves\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED891CB-9DF8-4EA4-9F0B-4A60D5F56B82}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA7FFA7-ECB6-4DBF-8C24-1FB169DFB6A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3135" windowWidth="21645" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="3105" windowWidth="21645" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4854" uniqueCount="4520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="4523">
   <si>
     <t>Ash'ana</t>
   </si>
@@ -13580,6 +13580,15 @@
   </si>
   <si>
     <t>2371</t>
+  </si>
+  <si>
+    <t>Trecker</t>
+  </si>
+  <si>
+    <t>2539</t>
+  </si>
+  <si>
+    <t>81028724</t>
   </si>
 </sst>
 </file>
@@ -13615,8 +13624,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13956,10 +13966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1618"/>
+  <dimension ref="A1:C1619"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A1611" workbookViewId="0">
+      <selection activeCell="D1618" sqref="D1618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -31767,6 +31777,17 @@
         <v>3484</v>
       </c>
     </row>
+    <row r="1619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1619" t="s">
+        <v>4520</v>
+      </c>
+      <c r="B1619" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="C1619" s="1" t="s">
+        <v>4522</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>